<commit_message>
Registration Datadriven Test updated
</commit_message>
<xml_diff>
--- a/src/main/TestData.xlsx
+++ b/src/main/TestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7620"/>
+    <workbookView windowWidth="19035" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="Rgeistration Page " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
   <si>
     <t>Username</t>
   </si>
@@ -129,6 +130,174 @@
   </si>
   <si>
     <t>Special!@#123</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>john.doe@example.com</t>
+  </si>
+  <si>
+    <t>Password123</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>priya.sharma@example.com</t>
+  </si>
+  <si>
+    <t>SecurePass456</t>
+  </si>
+  <si>
+    <t>Amit</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>amit.kumar@example.com</t>
+  </si>
+  <si>
+    <t>AmitPass789</t>
+  </si>
+  <si>
+    <t>john.doe@</t>
+  </si>
+  <si>
+    <t>priya@@example.com</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>Aarti</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>aarti.singh@example.com</t>
+  </si>
+  <si>
+    <t>ValidPass1</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Verma</t>
+  </si>
+  <si>
+    <t>rahul.verma@example.com</t>
+  </si>
+  <si>
+    <t>StrongPass2024</t>
+  </si>
+  <si>
+    <t>Rahul123</t>
+  </si>
+  <si>
+    <t>Singh@</t>
+  </si>
+  <si>
+    <t>Vikram</t>
+  </si>
+  <si>
+    <t>Patel</t>
+  </si>
+  <si>
+    <t>vikram.patel@example.com</t>
+  </si>
+  <si>
+    <t>Pa$$word2024</t>
+  </si>
+  <si>
+    <t>Tara</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>tara.gupta@example.com</t>
+  </si>
+  <si>
+    <t>Tara2024</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>Malhotra</t>
+  </si>
+  <si>
+    <t>SunilPass</t>
+  </si>
+  <si>
+    <t>Neha</t>
+  </si>
+  <si>
+    <t>Joshi</t>
+  </si>
+  <si>
+    <t>neha.joshi@example.com</t>
+  </si>
+  <si>
+    <t>Jay</t>
+  </si>
+  <si>
+    <t>Mehta</t>
+  </si>
+  <si>
+    <t>jay.mehta@example.com</t>
+  </si>
+  <si>
+    <t>JayM@123</t>
+  </si>
+  <si>
+    <t>Anjali</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>anjali.roy@nope</t>
+  </si>
+  <si>
+    <t>Test1234</t>
+  </si>
+  <si>
+    <t>Manish</t>
+  </si>
+  <si>
+    <t>manish.sharma@example.com</t>
+  </si>
+  <si>
+    <t>manish</t>
   </si>
 </sst>
 </file>
@@ -141,7 +310,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,13 +320,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -633,161 +795,164 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -1111,15 +1276,15 @@
   <sheetPr/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.8571428571429" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.4285714285714" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24" style="4" customWidth="1"/>
+    <col min="2" max="2" width="23.8571428571429" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.4285714285714" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1154,7 +1319,7 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
@@ -1374,4 +1539,392 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="7.42857142857143" style="1" customWidth="1"/>
+    <col min="2" max="3" width="8.71428571428571" style="1" customWidth="1"/>
+    <col min="4" max="5" width="9.14285714285714" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="45" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" ht="60" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" ht="45" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" ht="45" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" ht="60" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" ht="30" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" ht="45" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" ht="45" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" ht="45" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" ht="60" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" ht="60" spans="1:5">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" ht="60" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" ht="45" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" ht="60" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" ht="45" spans="1:5">
+      <c r="A16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" ht="45" spans="1:5">
+      <c r="A18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" ht="45" spans="1:5">
+      <c r="A19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" ht="30" spans="1:5">
+      <c r="A20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" ht="60" spans="1:5">
+      <c r="A21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="john.doe@example.com" tooltip="mailto:john.doe@example.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="priya.sharma@example.com" tooltip="mailto:priya.sharma@example.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="amit.kumar@example.com" tooltip="mailto:amit.kumar@example.com"/>
+    <hyperlink ref="D5" r:id="rId3" display="amit.kumar@example.com" tooltip="mailto:amit.kumar@example.com"/>
+    <hyperlink ref="D6" r:id="rId2" display="priya.sharma@example.com" tooltip="mailto:priya.sharma@example.com"/>
+    <hyperlink ref="D9" r:id="rId1" display="john.doe@example.com" tooltip="mailto:john.doe@example.com"/>
+    <hyperlink ref="D10" r:id="rId4" display="aarti.singh@example.com" tooltip="mailto:aarti.singh@example.com"/>
+    <hyperlink ref="D11" r:id="rId5" display="rahul.verma@example.com" tooltip="mailto:rahul.verma@example.com"/>
+    <hyperlink ref="D12" r:id="rId5" display="rahul.verma@example.com" tooltip="mailto:rahul.verma@example.com"/>
+    <hyperlink ref="D13" r:id="rId5" display="rahul.verma@example.com" tooltip="mailto:rahul.verma@example.com"/>
+    <hyperlink ref="D14" r:id="rId4" display="aarti.singh@example.com" tooltip="mailto:aarti.singh@example.com"/>
+    <hyperlink ref="D15" r:id="rId6" display="vikram.patel@example.com" tooltip="mailto:vikram.patel@example.com"/>
+    <hyperlink ref="D16" r:id="rId7" display="tara.gupta@example.com" tooltip="mailto:tara.gupta@example.com"/>
+    <hyperlink ref="D18" r:id="rId8" display="neha.joshi@example.com" tooltip="mailto:neha.joshi@example.com"/>
+    <hyperlink ref="D19" r:id="rId9" display="jay.mehta@example.com" tooltip="mailto:jay.mehta@example.com"/>
+    <hyperlink ref="D21" r:id="rId10" display="manish.sharma@example.com" tooltip="mailto:manish.sharma@example.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>